<commit_message>
Updated project data file
</commit_message>
<xml_diff>
--- a/Sample_data_set.xlsx
+++ b/Sample_data_set.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Area/N2O</t>
   </si>
@@ -32,73 +32,91 @@
     <t>Quantity/N2O</t>
   </si>
   <si>
-    <t>2018\06\AIR CHK 262018_6_28_2018 7_13_50 PM.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404B_T4562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404B_T3062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404B_T1562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404B_T062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404_T4562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404_T3062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404_T1562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_404_T062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_403_T4562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_403_T3062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_403_T1562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_403_T062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_402_T4562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_402_T3062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_402_T1562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_402_T062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_401_T4562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_401_T3062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_401_T1562018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\COLBY_401_T062018.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\Standard Check_1_62018_6_28_2018 4_20_33 PM.DATA</t>
-  </si>
-  <si>
-    <t>2018\06\STD CHK 262018.DATA</t>
+    <t>2018\06\COLBY_304_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_304_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_304_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_304_T062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_303_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_303_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_303_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_303_T062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302B_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302B_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302B_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302B_T062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_302_T062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_301_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_301_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_301_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_301_T062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_204_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_204_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_204_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_204_T062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\STD CHK 262218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_203B_T4562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_203B_T3062218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_203B_T1562218.DATA</t>
+  </si>
+  <si>
+    <t>2018\06\COLBY_203B_T062218.DATA</t>
   </si>
 </sst>
 </file>
@@ -143,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -160,6 +178,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,278 +466,392 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="55.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8615.6</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2.42</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>1756.4</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B3" s="2">
+        <v>1750.1</v>
+      </c>
+      <c r="C3" s="5">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>1793.9</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B4" s="2">
+        <v>1771.6</v>
+      </c>
+      <c r="C4" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>2194.5</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2">
+        <v>1774.6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>2001.6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.56000000000000005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2">
+        <v>1750.6</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>1794.2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="2">
+        <v>5081.6000000000004</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.43</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
-        <v>2624.5</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="2">
+        <v>4473.5</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
-        <v>2354.5</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2">
+        <v>3076.3</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.87</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2">
-        <v>2019.7</v>
-      </c>
-      <c r="C9" s="5">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B10" s="2">
-        <v>1815.1</v>
+        <v>1803.3</v>
       </c>
       <c r="C10" s="5">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2209.6</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
-        <v>3275.8</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="2">
+        <v>2078.4</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
-        <v>1759</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B13" s="2">
+        <v>1904.7</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.54</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1772.7</v>
+      </c>
+      <c r="C14" s="5">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2310.9</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="2">
-        <v>1796.8</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="2">
+        <v>8211.2000000000007</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2.31</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
-        <v>6353.9</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="2">
+        <v>6340.8</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.78</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2">
-        <v>4949.2</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1.39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="2">
+        <v>3961.6</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2">
-        <v>3547.6</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B18" s="2">
-        <v>1796.1</v>
+        <v>1810.7</v>
       </c>
       <c r="C18" s="5">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>8548.7999999999993</v>
+      </c>
+      <c r="C19" s="5">
+        <v>2.41</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2">
-        <v>5439.5</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="2">
+        <v>7170.7</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2.02</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2">
-        <v>4601.8999999999996</v>
-      </c>
-      <c r="C20" s="2">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="2">
+        <v>4507.1000000000004</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1.27</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2">
-        <v>3461.1</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="4">
+        <v>1852.3</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="4">
-        <v>1838.5</v>
-      </c>
-      <c r="C22" s="4">
+      <c r="B23" s="2">
+        <v>1848.7</v>
+      </c>
+      <c r="C23" s="5">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2">
-        <v>8860.4</v>
-      </c>
-      <c r="C23" s="2">
-        <v>2.4900000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="2">
+        <v>1782.4</v>
+      </c>
+      <c r="C24" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2">
-        <v>8988.7000000000007</v>
-      </c>
-      <c r="C24" s="2">
-        <v>2.5299999999999998</v>
+      <c r="B25" s="2">
+        <v>1786.8</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1723.9</v>
+      </c>
+      <c r="C26" s="5">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2153.9</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2019.9</v>
+      </c>
+      <c r="C28" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1920</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1788.6</v>
+      </c>
+      <c r="C30" s="5">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>